<commit_message>
Removed zeros in the datasets Nconc - Casino and Gatton
</commit_message>
<xml_diff>
--- a/Tests/Validation/Ryegrass/CasinoObserved9194.xlsx
+++ b/Tests/Validation/Ryegrass/CasinoObserved9194.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jessica\GIT\ApsimX\ApsimX\Tests\Validation\Ryegrass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C14FB-D3FC-418D-9C0C-01B5367DC613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73614556-87CA-4A0E-97F1-98EC46162616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="81480" yWindow="15" windowWidth="38640" windowHeight="21120" xr2:uid="{D8D4DAC5-FC5C-46B1-A308-548BE785F036}"/>
+    <workbookView xWindow="43080" yWindow="-3975" windowWidth="38640" windowHeight="21120" xr2:uid="{D8D4DAC5-FC5C-46B1-A308-548BE785F036}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBBC250-8FE2-48DD-B4B3-8CAA37EE90E8}">
   <dimension ref="A1:E267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="K271" sqref="K271"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="K245" sqref="K245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2045,9 +2045,6 @@
       <c r="B123" s="2">
         <v>34599</v>
       </c>
-      <c r="C123">
-        <v>0</v>
-      </c>
       <c r="E123">
         <v>25</v>
       </c>
@@ -2557,9 +2554,6 @@
       </c>
       <c r="B165" s="2">
         <v>34599</v>
-      </c>
-      <c r="C165">
-        <v>0</v>
       </c>
       <c r="E165">
         <v>75</v>

</xml_diff>